<commit_message>
Continue to change structures, now i am changing the shop windows
</commit_message>
<xml_diff>
--- a/DataSource/excel/eventAction.xlsx
+++ b/DataSource/excel/eventAction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22740" yWindow="3740" windowWidth="29720" windowHeight="25120" tabRatio="500"/>
+    <workbookView xWindow="21480" yWindow="2000" windowWidth="29720" windowHeight="25120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="eventAction.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="379">
   <si>
     <t>id</t>
   </si>
@@ -485,18 +485,12 @@
     <t>hireSailorHireNumberChange</t>
   </si>
   <si>
-    <t>hireSailorCostMoney</t>
-  </si>
-  <si>
     <t>dataChange</t>
   </si>
   <si>
     <t>money;-;cache.money</t>
   </si>
   <si>
-    <t>hireSailorHireNumberChange;hireSailorCurrNumberChange;hireSailorCostMoney;waitADay;hireSailorFull</t>
-  </si>
-  <si>
     <t>水手快满了</t>
   </si>
   <si>
@@ -1034,15 +1028,9 @@
     <t>sleepMoneySuccessDialog</t>
   </si>
   <si>
-    <t>sleepMoneySuccessCostMoney</t>
-  </si>
-  <si>
     <t>sleepMoneySuccessCostDay</t>
   </si>
   <si>
-    <t>close;sleepMoneySuccessDialog;sleepMoneySuccessCostMoney;sleepMoneySuccessCostDay;inn</t>
-  </si>
-  <si>
     <t>dialog_have_a_good_sleep</t>
   </si>
   <si>
@@ -1116,6 +1104,66 @@
   </si>
   <si>
     <t>buyItemCancelSmallWindow</t>
+  </si>
+  <si>
+    <t>buyItemConfirmedDialogData</t>
+  </si>
+  <si>
+    <t>buyItemConfirmedMoney</t>
+  </si>
+  <si>
+    <t>money=item.money</t>
+  </si>
+  <si>
+    <t>item.itemName;cache.money</t>
+  </si>
+  <si>
+    <t>buyItemConfirmedDialog</t>
+  </si>
+  <si>
+    <t>buyItemConfirmedMoney;buyItemConfirmedDialogData;buyItemConfirmedDialog</t>
+  </si>
+  <si>
+    <t>dialog_buy_item;buyItemDealStart;buyItemDealCanceled</t>
+  </si>
+  <si>
+    <t>buyItemDealStart</t>
+  </si>
+  <si>
+    <t>buyItemDealCanceled</t>
+  </si>
+  <si>
+    <t>buyItemMoneyEnough</t>
+  </si>
+  <si>
+    <t>moneyEnough;buyItemSuccess;buyItemFailed</t>
+  </si>
+  <si>
+    <t>buyItemSuccess</t>
+  </si>
+  <si>
+    <t>buyItemFailed</t>
+  </si>
+  <si>
+    <t>moneyNotEnoughDialog;buyItemDealCanceled</t>
+  </si>
+  <si>
+    <t>costMoney</t>
+  </si>
+  <si>
+    <t>hireSailorHireNumberChange;hireSailorCurrNumberChange;costMoney;waitADay;hireSailorFull</t>
+  </si>
+  <si>
+    <t>close;sleepMoneySuccessDialog;costMoney;sleepMoneySuccessCostDay;inn</t>
+  </si>
+  <si>
+    <t>buyItemGainItem</t>
+  </si>
+  <si>
+    <t>item;get;reserved.itemId</t>
+  </si>
+  <si>
+    <t>costMoney;buyItemGainItem</t>
   </si>
 </sst>
 </file>
@@ -1525,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1611,7 +1659,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
@@ -1751,10 +1799,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>31</v>
@@ -1774,7 +1822,7 @@
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1788,7 +1836,7 @@
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1802,7 +1850,7 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1844,7 +1892,7 @@
         <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1852,18 +1900,18 @@
         <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>48</v>
@@ -1886,7 +1934,7 @@
         <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1922,18 +1970,18 @@
         <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>48</v>
@@ -1956,7 +2004,7 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1970,7 +2018,7 @@
         <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1984,7 +2032,7 @@
         <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2012,7 +2060,7 @@
         <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2024,7 +2072,7 @@
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2038,7 +2086,7 @@
         <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2057,7 +2105,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>90</v>
@@ -2066,7 +2114,7 @@
         <v>40</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2136,7 +2184,7 @@
         <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -2178,7 +2226,7 @@
         <v>41</v>
       </c>
       <c r="D46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2242,7 +2290,7 @@
         <v>41</v>
       </c>
       <c r="D51" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2254,7 +2302,7 @@
         <v>40</v>
       </c>
       <c r="D52" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2266,7 +2314,7 @@
         <v>41</v>
       </c>
       <c r="D53" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2274,7 +2322,7 @@
         <v>135</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>40</v>
@@ -2316,7 +2364,7 @@
         <v>147</v>
       </c>
       <c r="D57" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2324,7 +2372,7 @@
         <v>142</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>40</v>
@@ -2359,14 +2407,14 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D61" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2374,13 +2422,13 @@
         <v>148</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D62" t="s">
-        <v>155</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2409,14 +2457,14 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>373</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D65" t="s">
         <v>153</v>
-      </c>
-      <c r="D65" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2458,26 +2506,26 @@
         <v>54</v>
       </c>
       <c r="D68" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D69" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>42</v>
@@ -2486,110 +2534,110 @@
         <v>41</v>
       </c>
       <c r="D70" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D71" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D72" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D73" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D74" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D75" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D76" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D77" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>64</v>
@@ -2598,253 +2646,253 @@
         <v>40</v>
       </c>
       <c r="D78" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D79" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>208</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="D80" t="s">
         <v>211</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D80" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D81" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D82" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D84" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D85" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D86" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D87" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D88" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>234</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D89" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D90" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D91" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D92" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D93" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D94" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>244</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D95" t="s">
         <v>246</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D95" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>40</v>
@@ -2855,76 +2903,76 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>251</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D97" t="s">
         <v>253</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D97" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D98" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D99" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D100" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D101" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D102" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>40</v>
@@ -2935,7 +2983,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>40</v>
@@ -2946,76 +2994,76 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B105" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D105" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D106" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D107" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D108" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D109" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D110" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>40</v>
@@ -3026,7 +3074,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>40</v>
@@ -3037,76 +3085,76 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B113" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D113" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D114" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D115" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D116" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D117" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D118" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>40</v>
@@ -3117,7 +3165,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>40</v>
@@ -3128,7 +3176,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B121" t="s">
         <v>18</v>
@@ -3137,252 +3185,252 @@
         <v>54</v>
       </c>
       <c r="D121" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B122" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D122" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D123" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D124" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D125" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D126" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D127" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D128" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D129" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D130" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D131" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D132" t="s">
-        <v>337</v>
+        <v>375</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D133" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>333</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D134" t="s">
         <v>335</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D134" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D135" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D136" t="s">
-        <v>341</v>
+        <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>340</v>
+        <v>338</v>
+      </c>
+      <c r="B137" t="s">
+        <v>339</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>153</v>
+        <v>40</v>
       </c>
       <c r="D137" t="s">
-        <v>60</v>
+        <v>356</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>342</v>
-      </c>
-      <c r="B138" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D138" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D139" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D140" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D141" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D142" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D143" t="s">
         <v>348</v>
@@ -3390,51 +3438,51 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D144" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D145" t="s">
-        <v>358</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D146" t="s">
-        <v>7</v>
+        <v>355</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D147" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>40</v>
@@ -3445,13 +3493,101 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>360</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D149" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>359</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D150" t="s">
         <v>362</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D149" t="s">
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>363</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D151" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>366</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D152" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>367</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D153" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>368</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D154" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>370</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D155" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>371</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D156" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>376</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D157" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue to change structure -- change equip view...
</commit_message>
<xml_diff>
--- a/DataSource/excel/eventAction.xlsx
+++ b/DataSource/excel/eventAction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="3260" windowWidth="29720" windowHeight="25120" tabRatio="500"/>
+    <workbookView xWindow="47860" yWindow="6540" windowWidth="28800" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="eventAction.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="466">
   <si>
     <t>id</t>
   </si>
@@ -1266,6 +1266,165 @@
   </si>
   <si>
     <t>分配水手</t>
+  </si>
+  <si>
+    <t>infoList</t>
+  </si>
+  <si>
+    <t>情报</t>
+  </si>
+  <si>
+    <t>shipInfo</t>
+  </si>
+  <si>
+    <t>itemInfo</t>
+  </si>
+  <si>
+    <t>taskInfo</t>
+  </si>
+  <si>
+    <t>npcInfo</t>
+  </si>
+  <si>
+    <t>diaryInfo</t>
+  </si>
+  <si>
+    <t>npcInfo;shipInfo;itemInfo;taskInfo;diaryInfo;close</t>
+  </si>
+  <si>
+    <t>船员情报</t>
+  </si>
+  <si>
+    <t>船只情报</t>
+  </si>
+  <si>
+    <t>持有道具</t>
+  </si>
+  <si>
+    <t>任务资讯</t>
+  </si>
+  <si>
+    <t>航海日志</t>
+  </si>
+  <si>
+    <t>deckArrange</t>
+  </si>
+  <si>
+    <t>甲板</t>
+  </si>
+  <si>
+    <t>systemList</t>
+  </si>
+  <si>
+    <t>系统</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>systemSetting</t>
+  </si>
+  <si>
+    <t>save;load;systemSetting;close</t>
+  </si>
+  <si>
+    <t>sailMap</t>
+  </si>
+  <si>
+    <t>航海图</t>
+  </si>
+  <si>
+    <t>close;itemInfoWindow</t>
+  </si>
+  <si>
+    <t>itemInfoWindow</t>
+  </si>
+  <si>
+    <t>ItemBrowsePanel;browseItemSelected;infoList;2</t>
+  </si>
+  <si>
+    <t>browseItemSelected</t>
+  </si>
+  <si>
+    <t>ItemInfoPanel;itemUseSelected;itemInfoWindow;2;reserved.itemId</t>
+  </si>
+  <si>
+    <t>itemUseSelected</t>
+  </si>
+  <si>
+    <t>使用/装备道具</t>
+  </si>
+  <si>
+    <t>ProgressPanel;;;0</t>
+  </si>
+  <si>
+    <t>ProgressPanel;;;1</t>
+  </si>
+  <si>
+    <t>deckArrangeHaveShip</t>
+  </si>
+  <si>
+    <t>haveShip;deckArrangeWindow;deckArrangeFailedDialog</t>
+  </si>
+  <si>
+    <t>deckArrangeFailedDialog</t>
+  </si>
+  <si>
+    <t>deckArrangeWindow</t>
+  </si>
+  <si>
+    <t>ShipPanel;;;0</t>
+  </si>
+  <si>
+    <t>close;haveShipModify</t>
+  </si>
+  <si>
+    <t>modifyShipNoShip</t>
+  </si>
+  <si>
+    <t>modifyShipNoShipDialog;shipyard</t>
+  </si>
+  <si>
+    <t>ShipPanel;shipyard;modifyShipWindow;1</t>
+  </si>
+  <si>
+    <t>ShipInfoWindow</t>
+  </si>
+  <si>
+    <t>ShipExchangePanel;ShipInfoWindow;;3</t>
+  </si>
+  <si>
+    <t>ShipPanel;;;3</t>
+  </si>
+  <si>
+    <t>RolePanel;;;0</t>
+  </si>
+  <si>
+    <t>itemIsEquip</t>
+  </si>
+  <si>
+    <t>itemIsEquip;</t>
+  </si>
+  <si>
+    <t>itemEquipRolePanel</t>
+  </si>
+  <si>
+    <t>itemEquipSuccess</t>
+  </si>
+  <si>
+    <t>RolePanel;itemEquipSuccess;browseItemSelected;1</t>
+  </si>
+  <si>
+    <t>itemEquipSuccessDialog</t>
+  </si>
+  <si>
+    <t>itemEquipSuccessDialog;browseItemSelected</t>
+  </si>
+  <si>
+    <t>dialog_equip_an_equipment_success</t>
   </si>
 </sst>
 </file>
@@ -1675,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B168" sqref="B168"/>
+    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3196,7 +3355,7 @@
         <v>40</v>
       </c>
       <c r="D113" t="s">
-        <v>273</v>
+        <v>450</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -3212,699 +3371,1003 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>274</v>
+        <v>451</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D115" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D116" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D117" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D118" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D119" t="s">
-        <v>124</v>
+        <v>291</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D120" t="s">
-        <v>124</v>
+        <v>453</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>292</v>
-      </c>
-      <c r="B121" t="s">
-        <v>18</v>
+        <v>281</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D121" t="s">
-        <v>293</v>
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="B122" t="s">
-        <v>314</v>
+        <v>18</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D122" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>312</v>
+        <v>309</v>
+      </c>
+      <c r="B123" t="s">
+        <v>314</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D123" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D124" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D125" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D126" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D127" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D128" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D129" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D130" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="D131" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D132" t="s">
-        <v>373</v>
+        <v>331</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D133" t="s">
-        <v>334</v>
+        <v>373</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="D134" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D135" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D136" t="s">
-        <v>60</v>
+        <v>337</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>338</v>
-      </c>
-      <c r="B137" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D137" t="s">
-        <v>356</v>
+        <v>60</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>340</v>
+        <v>338</v>
+      </c>
+      <c r="B138" t="s">
+        <v>339</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D138" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D139" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D140" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D141" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D142" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D143" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D144" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D145" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D146" t="s">
-        <v>355</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D147" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D148" t="s">
-        <v>345</v>
+        <v>395</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>394</v>
+        <v>358</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D149" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>359</v>
+        <v>394</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D150" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D151" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="D152" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D153" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D154" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D155" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D156" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>152</v>
+        <v>40</v>
       </c>
       <c r="D157" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>377</v>
-      </c>
-      <c r="B158" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="D158" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>380</v>
+        <v>377</v>
+      </c>
+      <c r="B159" t="s">
+        <v>378</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D159" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D160" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D161" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D162" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D163" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D164" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>388</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D165" t="s">
         <v>390</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D165" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D166" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D167" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="D168" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="D169" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D170" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>152</v>
+        <v>40</v>
       </c>
       <c r="D171" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>152</v>
       </c>
       <c r="D172" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>406</v>
-      </c>
-      <c r="B173" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="D173" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>406</v>
+      </c>
+      <c r="B174" t="s">
+        <v>412</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D174" t="s">
         <v>407</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D174" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D175" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>408</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D176" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>409</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C177" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D177" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>413</v>
+      </c>
+      <c r="B178" t="s">
+        <v>414</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D178" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>418</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D179" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>415</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D180" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>454</v>
+      </c>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D181" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>416</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D182" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>437</v>
+      </c>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D183" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>439</v>
+      </c>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D184" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>441</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D185" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>458</v>
+      </c>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D186" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>460</v>
+      </c>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D187" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>461</v>
+      </c>
+      <c r="B188" s="1"/>
+      <c r="C188" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D188" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>463</v>
+      </c>
+      <c r="B189" s="1"/>
+      <c r="C189" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D189" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>417</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D190" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>419</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D191" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>426</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D192" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>445</v>
+      </c>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D193" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>448</v>
+      </c>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D194" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>447</v>
+      </c>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D195" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>428</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C196" t="s">
+        <v>23</v>
+      </c>
+      <c r="D196" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>430</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D197" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>431</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D198" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>432</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D199" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>434</v>
+      </c>
+      <c r="B200" t="s">
+        <v>435</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D200" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task data panel's completion
</commit_message>
<xml_diff>
--- a/DataSource/excel/eventAction.xlsx
+++ b/DataSource/excel/eventAction.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="2960" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="1920" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="eventAction.csv" sheetId="1" r:id="rId1"/>
@@ -1868,9 +1868,6 @@
     <t>取消任务</t>
   </si>
   <si>
-    <t>TaskPanel;shop;cityTasksShowUp;1</t>
-  </si>
-  <si>
     <t>cancelTaskDialog</t>
   </si>
   <si>
@@ -1989,6 +1986,9 @@
   </si>
   <si>
     <t>cityHasNoTasksDialog;shop</t>
+  </si>
+  <si>
+    <t>TaskPanel;shop;cityTasksShowUp;0</t>
   </si>
 </sst>
 </file>
@@ -2456,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D274" sqref="D274"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B265" sqref="B265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5364,7 +5364,7 @@
         <v>39</v>
       </c>
       <c r="D230" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -5492,26 +5492,26 @@
         <v>141</v>
       </c>
       <c r="D240" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
+        <v>615</v>
+      </c>
+      <c r="B241" t="s">
         <v>616</v>
       </c>
-      <c r="B241" t="s">
-        <v>617</v>
-      </c>
       <c r="C241" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D241" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B242" t="s">
         <v>531</v>
@@ -5520,68 +5520,68 @@
         <v>40</v>
       </c>
       <c r="D242" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D243" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
+        <v>630</v>
+      </c>
+      <c r="B244" t="s">
         <v>631</v>
       </c>
-      <c r="B244" t="s">
-        <v>632</v>
-      </c>
       <c r="C244" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D244" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
+        <v>634</v>
+      </c>
+      <c r="B245" t="s">
         <v>635</v>
-      </c>
-      <c r="B245" t="s">
-        <v>636</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D245" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D246" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D247" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -5650,7 +5650,7 @@
         <v>39</v>
       </c>
       <c r="D253" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
@@ -5666,7 +5666,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>146</v>
@@ -5683,7 +5683,7 @@
         <v>39</v>
       </c>
       <c r="D256" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
@@ -5710,16 +5710,16 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
+        <v>623</v>
+      </c>
+      <c r="B259" t="s">
         <v>624</v>
-      </c>
-      <c r="B259" t="s">
-        <v>625</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D259" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
@@ -5892,7 +5892,7 @@
         <v>39</v>
       </c>
       <c r="D273" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
@@ -5903,7 +5903,7 @@
         <v>31</v>
       </c>
       <c r="D274" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
@@ -5925,7 +5925,7 @@
         <v>53</v>
       </c>
       <c r="D276" t="s">
-        <v>613</v>
+        <v>653</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
@@ -5939,23 +5939,23 @@
         <v>39</v>
       </c>
       <c r="D277" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D278" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>126</v>
@@ -5966,40 +5966,40 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D280" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D281" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D282" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>146</v>
@@ -6010,13 +6010,13 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D284" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some task bugs, and enable task review, save, load
</commit_message>
<xml_diff>
--- a/DataSource/excel/eventAction.xlsx
+++ b/DataSource/excel/eventAction.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="664">
   <si>
     <t>id</t>
   </si>
@@ -1989,6 +1989,36 @@
   </si>
   <si>
     <t>TaskPanel;shop;cityTasksShowUp;0</t>
+  </si>
+  <si>
+    <t>taskInfoHasTask</t>
+  </si>
+  <si>
+    <t>接取了任务</t>
+  </si>
+  <si>
+    <t>taskInfoShowCurrentTask</t>
+  </si>
+  <si>
+    <t>taskInfoDialogNoTask</t>
+  </si>
+  <si>
+    <t>hasTask;taskInfoShowCurrentTask;taskInfoNoTask</t>
+  </si>
+  <si>
+    <t>taskInfoNoTask</t>
+  </si>
+  <si>
+    <t>taskInfoDialogNoTask;infoList</t>
+  </si>
+  <si>
+    <t>dialog_no_task_received</t>
+  </si>
+  <si>
+    <t>closeWindow;taskInfoHasTask</t>
+  </si>
+  <si>
+    <t>TaskPanel;infoList;infoList;1</t>
   </si>
 </sst>
 </file>
@@ -2454,10 +2484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D284"/>
+  <dimension ref="A1:D288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B265" sqref="B265"/>
+    <sheetView tabSelected="1" topLeftCell="B202" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5172,850 +5202,900 @@
         <v>39</v>
       </c>
       <c r="D215" t="s">
-        <v>27</v>
+        <v>662</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>399</v>
+        <v>654</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>405</v>
+        <v>655</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D216" t="s">
-        <v>27</v>
+        <v>658</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>406</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>407</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="B217" s="1"/>
       <c r="C217" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D217" t="s">
-        <v>422</v>
+        <v>663</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>422</v>
+        <v>659</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D218" t="s">
-        <v>423</v>
+        <v>660</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>425</v>
+        <v>657</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D219" t="s">
-        <v>426</v>
+        <v>661</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>424</v>
-      </c>
-      <c r="B220" s="1"/>
+        <v>399</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="C220" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D220" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C221" t="s">
-        <v>23</v>
+        <v>407</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D221" t="s">
-        <v>585</v>
+        <v>422</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>410</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="B222" s="1"/>
       <c r="C222" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D222" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>411</v>
-      </c>
+        <v>425</v>
+      </c>
+      <c r="B223" s="1"/>
       <c r="C223" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D223" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>586</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="B224" s="1"/>
       <c r="C224" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D224" t="s">
-        <v>591</v>
+        <v>86</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>590</v>
+        <v>408</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>141</v>
+        <v>409</v>
+      </c>
+      <c r="C225" t="s">
+        <v>23</v>
       </c>
       <c r="D225" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>587</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>587</v>
+        <v>410</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>589</v>
+        <v>53</v>
       </c>
       <c r="D226" t="s">
-        <v>27</v>
+        <v>420</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D227" t="s">
-        <v>27</v>
+        <v>421</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>413</v>
-      </c>
-      <c r="B228" t="s">
-        <v>414</v>
+        <v>586</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>512</v>
+        <v>39</v>
       </c>
       <c r="D228" t="s">
-        <v>513</v>
+        <v>591</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>514</v>
-      </c>
-      <c r="B229" t="s">
-        <v>515</v>
+        <v>590</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>588</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>512</v>
+        <v>141</v>
       </c>
       <c r="D229" t="s">
-        <v>518</v>
+        <v>592</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>516</v>
-      </c>
-      <c r="B230" t="s">
-        <v>520</v>
+        <v>587</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>587</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>39</v>
+        <v>589</v>
       </c>
       <c r="D230" t="s">
-        <v>622</v>
+        <v>27</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>521</v>
-      </c>
-      <c r="B231" t="s">
-        <v>523</v>
+        <v>412</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D231" t="s">
-        <v>576</v>
+        <v>27</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>522</v>
+        <v>413</v>
       </c>
       <c r="B232" t="s">
-        <v>524</v>
+        <v>414</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>40</v>
+        <v>512</v>
       </c>
       <c r="D232" t="s">
-        <v>577</v>
+        <v>513</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="B233" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>40</v>
+        <v>512</v>
       </c>
       <c r="D233" t="s">
-        <v>546</v>
+        <v>518</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="B234" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D234" t="s">
-        <v>584</v>
+        <v>622</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>532</v>
+        <v>521</v>
+      </c>
+      <c r="B235" t="s">
+        <v>523</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D235" t="s">
-        <v>534</v>
+        <v>576</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>533</v>
+        <v>522</v>
+      </c>
+      <c r="B236" t="s">
+        <v>524</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D236" t="s">
-        <v>535</v>
+        <v>577</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>526</v>
+        <v>528</v>
+      </c>
+      <c r="B237" t="s">
+        <v>529</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D237" t="s">
-        <v>527</v>
+        <v>546</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>525</v>
+        <v>530</v>
+      </c>
+      <c r="B238" t="s">
+        <v>531</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D238" t="s">
-        <v>86</v>
+        <v>584</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>545</v>
-      </c>
-      <c r="B239" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="D239" t="s">
-        <v>580</v>
+        <v>534</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>548</v>
-      </c>
-      <c r="B240" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>141</v>
+        <v>31</v>
       </c>
       <c r="D240" t="s">
-        <v>626</v>
+        <v>535</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>615</v>
-      </c>
-      <c r="B241" t="s">
-        <v>616</v>
+        <v>526</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D241" t="s">
-        <v>629</v>
+        <v>527</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>627</v>
-      </c>
-      <c r="B242" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D242" t="s">
-        <v>632</v>
+        <v>86</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>628</v>
+        <v>545</v>
+      </c>
+      <c r="B243" t="s">
+        <v>547</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="D243" t="s">
-        <v>621</v>
+        <v>580</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>630</v>
+        <v>548</v>
       </c>
       <c r="B244" t="s">
-        <v>631</v>
+        <v>549</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="D244" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>634</v>
+        <v>615</v>
       </c>
       <c r="B245" t="s">
-        <v>635</v>
+        <v>616</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D245" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>620</v>
+        <v>627</v>
+      </c>
+      <c r="B246" t="s">
+        <v>531</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="D246" t="s">
-        <v>617</v>
+        <v>632</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>618</v>
+        <v>628</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="D247" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>536</v>
+        <v>630</v>
+      </c>
+      <c r="B248" t="s">
+        <v>631</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D248" t="s">
-        <v>582</v>
+        <v>633</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>538</v>
+        <v>634</v>
+      </c>
+      <c r="B249" t="s">
+        <v>635</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="D249" t="s">
-        <v>571</v>
+        <v>636</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>539</v>
+        <v>620</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="D250" t="s">
-        <v>537</v>
+        <v>617</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>581</v>
+        <v>618</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="D251" t="s">
-        <v>552</v>
+        <v>619</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D252" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>540</v>
-      </c>
-      <c r="B253" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="D253" t="s">
-        <v>639</v>
+        <v>571</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>575</v>
+        <v>539</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="D254" t="s">
-        <v>572</v>
+        <v>537</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>638</v>
+        <v>581</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D255" t="s">
-        <v>147</v>
+        <v>552</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D256" t="s">
-        <v>637</v>
+        <v>583</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>574</v>
+        <v>540</v>
+      </c>
+      <c r="B257" t="s">
+        <v>544</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="D257" t="s">
-        <v>573</v>
+        <v>639</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>543</v>
+        <v>575</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="D258" t="s">
-        <v>59</v>
+        <v>572</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>623</v>
-      </c>
-      <c r="B259" t="s">
-        <v>624</v>
+        <v>638</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="D259" t="s">
-        <v>625</v>
+        <v>147</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>550</v>
-      </c>
-      <c r="B260" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D260" t="s">
-        <v>564</v>
+        <v>637</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>553</v>
-      </c>
-      <c r="B261" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D261" t="s">
-        <v>555</v>
+        <v>573</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="D262" t="s">
-        <v>562</v>
+        <v>59</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>557</v>
+        <v>623</v>
       </c>
       <c r="B263" t="s">
-        <v>561</v>
+        <v>624</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D263" t="s">
-        <v>578</v>
+        <v>625</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>560</v>
+        <v>550</v>
+      </c>
+      <c r="B264" t="s">
+        <v>551</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D264" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>558</v>
+        <v>553</v>
+      </c>
+      <c r="B265" t="s">
+        <v>554</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="D265" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>559</v>
-      </c>
-      <c r="B266" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="D266" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>519</v>
+        <v>557</v>
+      </c>
+      <c r="B267" t="s">
+        <v>561</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>512</v>
+        <v>40</v>
       </c>
       <c r="D267" t="s">
-        <v>517</v>
+        <v>578</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>593</v>
-      </c>
-      <c r="B268" s="1" t="s">
-        <v>594</v>
+        <v>560</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D268" t="s">
-        <v>599</v>
+        <v>567</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>598</v>
-      </c>
-      <c r="B269" s="1"/>
+        <v>558</v>
+      </c>
       <c r="C269" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D269" t="s">
-        <v>595</v>
+        <v>565</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>596</v>
+        <v>559</v>
+      </c>
+      <c r="B270" t="s">
+        <v>556</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D270" t="s">
-        <v>605</v>
+        <v>566</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>603</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>604</v>
+        <v>519</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>606</v>
+        <v>512</v>
       </c>
       <c r="D271" t="s">
-        <v>7</v>
+        <v>517</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>600</v>
+        <v>593</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>594</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D272" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>597</v>
-      </c>
+        <v>598</v>
+      </c>
+      <c r="B273" s="1"/>
       <c r="C273" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D273" t="s">
-        <v>652</v>
+        <v>595</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D274" t="s">
-        <v>651</v>
+        <v>605</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>607</v>
+        <v>603</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>604</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>39</v>
+        <v>606</v>
       </c>
       <c r="D275" t="s">
-        <v>609</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D276" t="s">
-        <v>653</v>
+        <v>602</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>611</v>
-      </c>
-      <c r="B277" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D277" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>641</v>
+        <v>601</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="D278" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>644</v>
+        <v>607</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>126</v>
+        <v>39</v>
       </c>
       <c r="D279" t="s">
-        <v>537</v>
+        <v>609</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="D280" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>643</v>
+        <v>611</v>
+      </c>
+      <c r="B281" t="s">
+        <v>612</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D281" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="D282" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="D283" t="s">
-        <v>147</v>
+        <v>537</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
+        <v>613</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D284" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>643</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D285" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>645</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D286" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>647</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D287" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
         <v>614</v>
       </c>
-      <c r="C284" s="1" t="s">
+      <c r="C288" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D288" t="s">
         <v>640</v>
       </c>
     </row>

</xml_diff>